<commit_message>
Add login, register and some update data for user profile
</commit_message>
<xml_diff>
--- a/src/test/java/data/UserData.xlsx
+++ b/src/test/java/data/UserData.xlsx
@@ -5,31 +5,32 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\eclipse-workspace\hawyahUserApp\src\test\java\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\eclipse-workspace\hawyahUser\src\test\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71455DFE-4C05-4B96-8938-517B28F32371}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5C5163-8A75-4757-8B5D-15C50D7F1256}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginData" sheetId="1" r:id="rId1"/>
     <sheet name="AboutMeTest" sheetId="2" r:id="rId2"/>
     <sheet name="BasicIdentityTest" sheetId="3" r:id="rId3"/>
+    <sheet name="MessageTest" sheetId="4" r:id="rId4"/>
+    <sheet name="RequestDesignAndSearchTest" sheetId="5" r:id="rId5"/>
+    <sheet name="LoginUserTest" sheetId="6" r:id="rId6"/>
+    <sheet name="AboutMeDesignerTest" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>user url</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -54,9 +55,6 @@
     <t>confirmNewPass</t>
   </si>
   <si>
-    <t>إنغولا</t>
-  </si>
-  <si>
     <t>folderName</t>
   </si>
   <si>
@@ -67,6 +65,51 @@
   </si>
   <si>
     <t>الزراعة</t>
+  </si>
+  <si>
+    <t>email Cleint</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title </t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>Body Body Body</t>
+  </si>
+  <si>
+    <t>fromPrice</t>
+  </si>
+  <si>
+    <t>toPrice</t>
+  </si>
+  <si>
+    <t>ahmed.ali.hassan.elsetouhy@gmail.com</t>
+  </si>
+  <si>
+    <t>أنغولا</t>
+  </si>
+  <si>
+    <t>ibanNumber</t>
+  </si>
+  <si>
+    <t>accountOwnerName</t>
+  </si>
+  <si>
+    <t>bankAccount</t>
+  </si>
+  <si>
+    <t>"40055500000000001"</t>
+  </si>
+  <si>
+    <t>البنك المركزى المصري</t>
+  </si>
+  <si>
+    <t>محمد على</t>
   </si>
 </sst>
 </file>
@@ -432,12 +475,12 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
@@ -448,24 +491,24 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -486,7 +529,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,34 +540,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -536,7 +579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{068B593D-1783-4323-9FA8-42418A9B70FB}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -548,10 +591,111 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9CD383E-EF24-4D95-A12D-A481E0AA5D84}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B17DC1F-9038-4859-8877-E01D49082C86}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>40000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1C1484-B767-488E-A730-CC8922791BBD}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -559,7 +703,94 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{2155CB18-9072-461B-B130-E5357AC84779}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{25160C0C-614C-463E-BE3B-CBF3A916CD1E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E411ED3B-F4E2-49BD-82D8-2062E38451E8}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Designer profile test cases
</commit_message>
<xml_diff>
--- a/src/test/java/data/UserData.xlsx
+++ b/src/test/java/data/UserData.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\eclipse-workspace\hawyahUser\src\test\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035E9140-97B1-4A0A-8F93-F75E8CCD1A5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EB11A1-C51E-4913-B81E-08D92D51E4F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginData" sheetId="1" r:id="rId1"/>
+    <sheet name="0-LoginData" sheetId="1" r:id="rId1"/>
     <sheet name="AboutMeTest" sheetId="2" r:id="rId2"/>
     <sheet name="BasicIdentityTest" sheetId="3" r:id="rId3"/>
     <sheet name="MessageTest" sheetId="4" r:id="rId4"/>
     <sheet name="RequestDesignAndSearchTest" sheetId="5" r:id="rId5"/>
     <sheet name="LoginUserTest" sheetId="6" r:id="rId6"/>
     <sheet name="AboutMeDesignerTest" sheetId="7" r:id="rId7"/>
+    <sheet name="7-MyWorkUserTest" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>user url</t>
   </si>
@@ -474,7 +475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -580,7 +581,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -727,7 +728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E411ED3B-F4E2-49BD-82D8-2062E38451E8}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -796,4 +797,30 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D5DE316-6AB5-4C42-9BA9-E418E406B9E5}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Messages modules test cases
</commit_message>
<xml_diff>
--- a/src/test/java/data/UserData.xlsx
+++ b/src/test/java/data/UserData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\eclipse-workspace\hawyahUser\src\test\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EB11A1-C51E-4913-B81E-08D92D51E4F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8320629-D178-45E2-829A-372EC1EAF42F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0-LoginData" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,17 @@
     <sheet name="BasicIdentityTest" sheetId="3" r:id="rId3"/>
     <sheet name="MessageTest" sheetId="4" r:id="rId4"/>
     <sheet name="RequestDesignAndSearchTest" sheetId="5" r:id="rId5"/>
-    <sheet name="LoginUserTest" sheetId="6" r:id="rId6"/>
+    <sheet name="5-LoginUserTest" sheetId="6" r:id="rId6"/>
     <sheet name="AboutMeDesignerTest" sheetId="7" r:id="rId7"/>
     <sheet name="7-MyWorkUserTest" sheetId="8" r:id="rId8"/>
+    <sheet name="8-Designs Options" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>user url</t>
   </si>
@@ -111,6 +112,12 @@
   </si>
   <si>
     <t>محمد على</t>
+  </si>
+  <si>
+    <t>Design Name</t>
+  </si>
+  <si>
+    <t>تصميم هوية أساسية</t>
   </si>
 </sst>
 </file>
@@ -475,7 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -681,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1C1484-B767-488E-A730-CC8922791BBD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -823,4 +830,30 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7359ED32-C729-4EAC-974E-EAE8A5D8B978}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Designer scenarios for my competitions
</commit_message>
<xml_diff>
--- a/src/test/java/data/UserData.xlsx
+++ b/src/test/java/data/UserData.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\eclipse-workspace\hawyahUser\src\test\java\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B25FBB7-FCC8-422E-A8CE-CB5A9A48A887}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{94999B6F-38B6-4CD8-9E0B-041368BE6652}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="23304" windowHeight="13224" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0-LoginData" sheetId="1" r:id="rId1"/>
@@ -25,6 +20,7 @@
     <sheet name="9-DeliverFInalWorkCompetitionsD" sheetId="14" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:K9"/>
 </workbook>
 </file>
 
@@ -716,7 +712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1C1484-B767-488E-A730-CC8922791BBD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -864,7 +860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7359ED32-C729-4EAC-974E-EAE8A5D8B978}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add contests part admin
</commit_message>
<xml_diff>
--- a/src/test/java/data/UserData.xlsx
+++ b/src/test/java/data/UserData.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{94999B6F-38B6-4CD8-9E0B-041368BE6652}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\eclipse-workspace\hawyahUser\src\test\java\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C024E0-7138-41C3-9DBE-99E57ED79DAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="23304" windowHeight="13224" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0-LoginData" sheetId="1" r:id="rId1"/>
@@ -18,14 +23,14 @@
     <sheet name="7-MyWorkUserTest" sheetId="8" r:id="rId8"/>
     <sheet name="8-Designs Options" sheetId="13" r:id="rId9"/>
     <sheet name="9-DeliverFInalWorkCompetitionsD" sheetId="14" r:id="rId10"/>
+    <sheet name="10-AdminLogin" sheetId="15" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K9"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>user url</t>
   </si>
@@ -115,12 +120,24 @@
   </si>
   <si>
     <t>تصميم هوية أساسية</t>
+  </si>
+  <si>
+    <t>emailAdmin</t>
+  </si>
+  <si>
+    <t>ahmadali@hawyah.com</t>
+  </si>
+  <si>
+    <t>11111111a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,9 +176,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -556,6 +574,53 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7E557D-810B-45A6-B431-AF7CDFB36E47}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{8663722A-C526-4515-85BF-F66C99D48155}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF26A3B0-80EC-46F6-9049-38EEB4095E85}">
   <dimension ref="A1:B4"/>
@@ -712,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1C1484-B767-488E-A730-CC8922791BBD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Modification of disable status and update contests data test cases
</commit_message>
<xml_diff>
--- a/src/test/java/data/UserData.xlsx
+++ b/src/test/java/data/UserData.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\eclipse-workspace\hawyahUser\src\test\java\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C024E0-7138-41C3-9DBE-99E57ED79DAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FF83689F-B917-4794-BFD0-FFA025B3C3A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="23280" windowHeight="13224" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0-LoginData" sheetId="1" r:id="rId1"/>
@@ -26,6 +21,7 @@
     <sheet name="10-AdminLogin" sheetId="15" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:G6"/>
 </workbook>
 </file>
 
@@ -497,7 +493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -578,7 +574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7E557D-810B-45A6-B431-AF7CDFB36E47}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>